<commit_message>
merged with latest from UW team's update
</commit_message>
<xml_diff>
--- a/formidable-client/assets/opendatakit.collect2/form-files/example/example.xlsx
+++ b/formidable-client/assets/opendatakit.collect2/form-files/example/example.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="144">
   <si>
     <t>type</t>
   </si>
@@ -127,44 +127,46 @@
     <t>not(selected(data('examples'), 'label_features'))</t>
   </si>
   <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>&lt;u&gt;Labels&lt;/u&gt; &lt;i&gt;can&lt;/i&gt; contain &lt;span style="color:red;"&gt;HTML&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>So can &lt;b&gt;hints&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>Labels can contain &amp;lt;img&amp;gt; and &amp;lt;audio&amp;gt; HTML tags, but it is often easier to add media via the image and audio columns.</t>
+  </si>
+  <si>
+    <t>audio/carrioncrow.mp3</t>
+  </si>
+  <si>
+    <t>img/dolphin.png</t>
+  </si>
+  <si>
     <t>text</t>
   </si>
   <si>
     <t>Enter your name</t>
   </si>
   <si>
-    <t>Please use your full name</t>
-  </si>
-  <si>
-    <t>note</t>
-  </si>
-  <si>
-    <t>{{#if name}}
+    <t>It will be used in the next question.</t>
+  </si>
+  <si>
+    <t>&lt;h3&gt;
+This label uses Handlesbars template features:
+&lt;/h3&gt;
+{{#if name}}
 Hello {{name}}!
 {{else}}
 Name not entered.
-{{/if}}
-This label is a handlesbars template.</t>
+{{/if}}</t>
   </si>
   <si>
     <t>Handlebars templates allow labels to change depending on the values previously entered.</t>
   </si>
   <si>
-    <t>&lt;u&gt;Labels&lt;/u&gt; &lt;i&gt;can&lt;/i&gt; contain &lt;span style="color:red;"&gt;HTML&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t>So can &lt;b&gt;hints&lt;/b&gt;</t>
-  </si>
-  <si>
-    <t>Labels can contain &amp;lt;img&amp;gt; and &amp;lt;audio&amp;gt; HTML tags, but it is often easier to add media via the image and audio columns.</t>
-  </si>
-  <si>
-    <t>audio/carrioncrow.mp3</t>
-  </si>
-  <si>
-    <t>img/dolphin.png</t>
-  </si>
-  <si>
     <t>label label_features_end</t>
   </si>
   <si>
@@ -204,16 +206,19 @@
     <t>When were you born?</t>
   </si>
   <si>
-    <t>data('born').getDay() === now().getDay() &amp;&amp; data('born').getMonth() === now().getMonth()</t>
+    <t>data('born') &amp;&amp; data('born').getDay() === now().getDay() &amp;&amp; data('born').getMonth() === now().getMonth()</t>
   </si>
   <si>
     <t>Happy Birthday!</t>
   </si>
   <si>
+    <t>This prompt shows how to use dates in fomulas.</t>
+  </si>
+  <si>
     <t>time</t>
   </si>
   <si>
-    <t>What time is it?</t>
+    <t>What time do you usually wake up?</t>
   </si>
   <si>
     <t>datetime</t>
@@ -291,6 +296,30 @@
     <t>label media_end</t>
   </si>
   <si>
+    <t>selected(data('examples'), 'prompt_link')</t>
+  </si>
+  <si>
+    <t>&lt;a href="{{promptLink "unreachable"}}"&gt;This is a link to another prompt&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>label prompt_link_return</t>
+  </si>
+  <si>
+    <t>goto unreachable_end</t>
+  </si>
+  <si>
+    <t>unreachable</t>
+  </si>
+  <si>
+    <t>This prompt is unreachable except by links.</t>
+  </si>
+  <si>
+    <t>goto prompt_link_return</t>
+  </si>
+  <si>
+    <t>label unreachable_end</t>
+  </si>
+  <si>
     <t>selected(data('examples'), 'custom_template')</t>
   </si>
   <si>
@@ -397,6 +426,12 @@
   </si>
   <si>
     <t>custom template</t>
+  </si>
+  <si>
+    <t>prompt_link</t>
+  </si>
+  <si>
+    <t>prompt linking</t>
   </si>
   <si>
     <t>setting</t>
@@ -563,7 +598,7 @@
       <c t="s" s="1" r="C1">
         <v>2</v>
       </c>
-      <c t="s" s="1" r="D1">
+      <c t="s" s="3" r="D1">
         <v>3</v>
       </c>
       <c t="s" s="1" r="E1">
@@ -709,49 +744,49 @@
       <c t="s" s="1" r="A14">
         <v>37</v>
       </c>
-      <c t="s" s="1" r="C14">
-        <v>2</v>
-      </c>
-      <c t="s" s="1" r="D14">
+      <c t="s" r="D14">
         <v>38</v>
       </c>
-      <c t="s" s="1" r="E14">
+      <c t="s" r="E14">
         <v>39</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
+        <v>37</v>
+      </c>
+      <c t="s" s="3" r="D15">
         <v>40</v>
       </c>
-      <c t="s" s="1" r="D15">
+      <c t="s" s="1" r="G15">
         <v>41</v>
       </c>
-      <c t="s" r="E15">
+      <c t="s" s="1" r="H15">
         <v>42</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>40</v>
-      </c>
-      <c t="s" r="D16">
         <v>43</v>
       </c>
-      <c t="s" r="E16">
+      <c t="s" s="1" r="C16">
+        <v>2</v>
+      </c>
+      <c t="s" s="3" r="D16">
         <v>44</v>
+      </c>
+      <c t="s" s="1" r="E16">
+        <v>45</v>
       </c>
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c t="s" s="3" r="D17">
-        <v>45</v>
-      </c>
-      <c t="s" s="1" r="G17">
         <v>46</v>
       </c>
-      <c t="s" s="1" r="H17">
+      <c t="s" r="E17">
         <v>47</v>
       </c>
     </row>
@@ -806,46 +841,49 @@
       <c t="s" r="C22">
         <v>59</v>
       </c>
-      <c t="s" s="1" r="D22">
+      <c t="s" s="3" r="D22">
         <v>60</v>
       </c>
     </row>
     <row customHeight="1" r="23" ht="18.0">
       <c t="s" s="1" r="A23">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c t="s" r="B23">
         <v>61</v>
       </c>
-      <c t="s" s="1" r="D23">
+      <c t="s" s="3" r="D23">
         <v>62</v>
+      </c>
+      <c t="s" r="E23">
+        <v>63</v>
       </c>
     </row>
     <row customHeight="1" r="24" ht="18.0">
       <c t="s" s="1" r="A24">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c t="s" r="C24">
-        <v>63</v>
-      </c>
-      <c t="s" s="1" r="D24">
         <v>64</v>
+      </c>
+      <c t="s" s="3" r="D24">
+        <v>65</v>
       </c>
     </row>
     <row r="25">
       <c t="s" s="1" r="A25">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c t="s" s="1" r="C25">
-        <v>65</v>
-      </c>
-      <c t="s" s="1" r="D25">
         <v>66</v>
+      </c>
+      <c t="s" s="3" r="D25">
+        <v>67</v>
       </c>
     </row>
     <row customHeight="1" r="26" ht="18.0">
       <c t="s" s="4" r="A26">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c s="1" r="C26"/>
     </row>
@@ -854,32 +892,32 @@
         <v>28</v>
       </c>
       <c t="s" r="B27">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c t="s" s="1" r="C27">
-        <v>69</v>
-      </c>
-      <c t="s" s="1" r="D27">
         <v>70</v>
+      </c>
+      <c t="s" s="3" r="D27">
+        <v>71</v>
       </c>
     </row>
     <row r="28">
       <c t="s" s="1" r="A28">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c t="s" r="B28">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29">
       <c t="s" s="1" r="A29">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c t="s" s="1" r="C29">
-        <v>74</v>
-      </c>
-      <c t="s" s="1" r="D29">
         <v>75</v>
+      </c>
+      <c t="s" s="3" r="D29">
+        <v>76</v>
       </c>
     </row>
     <row r="30">
@@ -887,13 +925,13 @@
         <v>18</v>
       </c>
       <c t="s" s="1" r="B30">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c t="s" s="1" r="C30">
-        <v>77</v>
-      </c>
-      <c t="s" s="1" r="D30">
         <v>78</v>
+      </c>
+      <c t="s" s="3" r="D30">
+        <v>79</v>
       </c>
       <c t="b" r="M30">
         <v>1</v>
@@ -901,20 +939,20 @@
     </row>
     <row r="31">
       <c t="s" s="1" r="A31">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32">
       <c t="s" s="5" r="A32">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c t="s" r="B32">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33">
       <c t="s" s="1" r="A33">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34">
@@ -922,21 +960,21 @@
         <v>6</v>
       </c>
       <c t="s" s="1" r="C34">
-        <v>82</v>
-      </c>
-      <c t="s" s="1" r="D34">
         <v>83</v>
+      </c>
+      <c t="s" s="3" r="D34">
+        <v>84</v>
       </c>
     </row>
     <row r="35">
       <c t="s" s="1" r="A35">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c t="s" s="1" r="C35">
-        <v>85</v>
-      </c>
-      <c t="s" s="1" r="D35">
         <v>86</v>
+      </c>
+      <c t="s" s="3" r="D35">
+        <v>87</v>
       </c>
     </row>
     <row r="36">
@@ -944,63 +982,109 @@
         <v>7</v>
       </c>
       <c t="s" s="1" r="C36">
-        <v>87</v>
-      </c>
-      <c t="s" s="1" r="D36">
         <v>88</v>
+      </c>
+      <c t="s" s="3" r="D36">
+        <v>89</v>
       </c>
     </row>
     <row r="37">
       <c t="s" s="1" r="A37">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38">
       <c t="s" s="4" r="A38">
-        <v>89</v>
-      </c>
-      <c s="1" r="D38"/>
+        <v>90</v>
+      </c>
+      <c s="3" r="D38"/>
     </row>
     <row r="39">
       <c t="s" s="1" r="A39">
         <v>37</v>
       </c>
       <c t="s" r="B39">
-        <v>90</v>
-      </c>
-      <c t="s" s="1" r="C39">
         <v>91</v>
       </c>
-      <c t="s" s="1" r="D39">
+      <c t="s" s="3" r="D39">
         <v>92</v>
       </c>
-      <c t="s" s="1" r="I39">
+    </row>
+    <row r="40">
+      <c t="s" s="4" r="A40">
         <v>93</v>
       </c>
-    </row>
-    <row r="40">
-      <c t="s" s="1" r="A40">
+      <c s="3" r="D40"/>
+    </row>
+    <row r="41">
+      <c t="s" s="5" r="A41">
+        <v>94</v>
+      </c>
+      <c s="3" r="D41"/>
+    </row>
+    <row r="42">
+      <c t="s" s="1" r="A42">
+        <v>37</v>
+      </c>
+      <c t="s" r="C42">
+        <v>95</v>
+      </c>
+      <c t="s" s="3" r="D42">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43">
+      <c t="s" s="5" r="A43">
+        <v>97</v>
+      </c>
+      <c s="3" r="D43"/>
+    </row>
+    <row r="44">
+      <c t="s" s="4" r="A44">
+        <v>98</v>
+      </c>
+      <c s="3" r="D44"/>
+    </row>
+    <row r="45">
+      <c t="s" s="1" r="A45">
+        <v>43</v>
+      </c>
+      <c t="s" r="B45">
+        <v>99</v>
+      </c>
+      <c t="s" s="1" r="C45">
+        <v>100</v>
+      </c>
+      <c t="s" s="3" r="D45">
+        <v>101</v>
+      </c>
+      <c t="s" s="1" r="I45">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46">
+      <c t="s" s="1" r="A46">
         <v>49</v>
       </c>
-      <c t="s" s="1" r="C40">
-        <v>94</v>
-      </c>
-      <c t="s" s="1" r="D40">
-        <v>95</v>
-      </c>
-      <c t="s" r="E40">
-        <v>96</v>
-      </c>
-      <c r="F40">
+      <c t="s" s="1" r="C46">
+        <v>103</v>
+      </c>
+      <c t="s" s="3" r="D46">
+        <v>104</v>
+      </c>
+      <c t="s" r="E46">
+        <v>105</v>
+      </c>
+      <c r="F46">
         <v>5</v>
       </c>
-      <c t="s" s="1" r="J40">
-        <v>97</v>
-      </c>
-      <c s="1" r="K40">
+      <c t="s" s="1" r="J46">
+        <v>106</v>
+      </c>
+      <c s="1" r="K46">
         <v>1</v>
       </c>
-      <c s="1" r="L40">
+      <c s="1" r="L46">
         <v>10</v>
       </c>
     </row>
@@ -1024,15 +1108,15 @@
         <v>2</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>98</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>100</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1052,7 +1136,7 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c t="s" s="1" r="B1">
         <v>2</v>
@@ -1063,101 +1147,101 @@
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c t="s" s="1" r="C2">
-        <v>103</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>104</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c t="s" s="1" r="C4">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c t="s" s="1" r="C5">
-        <v>109</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c t="s" s="1" r="B6">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c t="s" s="1" r="C6">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c t="s" s="1" r="C7">
-        <v>111</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c t="s" s="1" r="B8">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c t="s" s="1" r="C8">
-        <v>112</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c t="s" s="1" r="B9">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c t="s" s="1" r="C9">
-        <v>113</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c t="s" s="1" r="B10">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c t="s" s="1" r="C10">
-        <v>114</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12">
@@ -1176,10 +1260,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B13">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c t="s" r="C13">
-        <v>116</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14">
@@ -1187,10 +1271,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B14">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c t="s" r="C14">
-        <v>118</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15">
@@ -1198,10 +1282,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B15">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c t="s" r="C15">
-        <v>120</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16">
@@ -1209,10 +1293,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B16">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c t="s" r="C16">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17">
@@ -1231,10 +1315,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B18">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c t="s" r="C18">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19">
@@ -1242,10 +1326,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B19">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c t="s" r="C19">
-        <v>123</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20">
@@ -1253,10 +1337,21 @@
         <v>14</v>
       </c>
       <c t="s" r="B20">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c t="s" r="C20">
-        <v>125</v>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21">
+      <c t="s" r="A21">
+        <v>14</v>
+      </c>
+      <c t="s" r="B21">
+        <v>135</v>
+      </c>
+      <c t="s" r="C21">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1275,23 +1370,23 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>127</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>129</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c s="1" r="B3">
         <v>1</v>
@@ -1299,10 +1394,10 @@
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>132</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>